<commit_message>
updated README file (updated table with overview of materials, link to MagNet, comma mistake) included a second function to calculate BH-integral (np.trapezoid)
</commit_message>
<xml_diff>
--- a/docs/source/figures/Material_Database_Overview.xlsx
+++ b/docs/source/figures/Material_Database_Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schacht\PycharmProjects\materialdatabase\docs\source\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14F2A7C-F93F-4AE0-8E52-A152E9ED685C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899237BE-9BC8-4042-BB71-301E75171A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E51A1F85-B08D-41FE-9B94-BB5FD5A5BD95}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>Material</t>
   </si>
@@ -217,16 +217,13 @@
     <t>LEA_LK*</t>
   </si>
   <si>
-    <t>LEA_MTB**</t>
-  </si>
-  <si>
-    <t>* former scientific worker of the LEA department</t>
-  </si>
-  <si>
-    <t>** own developt Material-Test-Bench by LEA department</t>
-  </si>
-  <si>
     <t>Proterial</t>
+  </si>
+  <si>
+    <t>LEA_MTB*</t>
+  </si>
+  <si>
+    <t>*measurements from department Power Electronics and Electrical Drives at Paderborn University</t>
   </si>
 </sst>
 </file>
@@ -708,13 +705,19 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -727,12 +730,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1078,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83654C4-16D0-484A-BE01-4B99138EE44B}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,8 +1084,9 @@
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="7.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="4" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="7" width="7" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
     <col min="9" max="9" width="25.42578125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
     <col min="11" max="11" width="25.7109375" customWidth="1"/>
@@ -1097,44 +1095,44 @@
     <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:16" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="47"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="50"/>
       <c r="H1" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="J1" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="48" t="s">
+      <c r="L1" s="51" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="47"/>
+    <row r="2" spans="1:16" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="42" t="s">
         <v>46</v>
       </c>
@@ -1150,10 +1148,10 @@
       <c r="H2" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="51"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="55"/>
     </row>
     <row r="3" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
@@ -1166,7 +1164,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="38"/>
       <c r="H3" s="45"/>
-      <c r="I3" s="49" t="s">
+      <c r="I3" s="48" t="s">
         <v>26</v>
       </c>
       <c r="J3" s="13">
@@ -1175,7 +1173,7 @@
       <c r="K3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="49" t="s">
+      <c r="L3" s="48" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1190,14 +1188,14 @@
       <c r="F4" s="33"/>
       <c r="G4" s="39"/>
       <c r="H4" s="46"/>
-      <c r="I4" s="49"/>
+      <c r="I4" s="48"/>
       <c r="J4" s="14">
         <v>2200</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="49"/>
+      <c r="L4" s="48"/>
     </row>
     <row r="5" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
@@ -1210,14 +1208,14 @@
       <c r="F5" s="33"/>
       <c r="G5" s="40"/>
       <c r="H5" s="46"/>
-      <c r="I5" s="49"/>
+      <c r="I5" s="48"/>
       <c r="J5" s="14">
         <v>1500</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="49"/>
+      <c r="L5" s="48"/>
     </row>
     <row r="6" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
@@ -1230,14 +1228,14 @@
       <c r="F6" s="33"/>
       <c r="G6" s="39"/>
       <c r="H6" s="33"/>
-      <c r="I6" s="49"/>
+      <c r="I6" s="48"/>
       <c r="J6" s="14">
         <v>800</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="49"/>
+      <c r="L6" s="48"/>
     </row>
     <row r="7" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
@@ -1250,14 +1248,14 @@
       <c r="F7" s="33"/>
       <c r="G7" s="39"/>
       <c r="H7" s="36"/>
-      <c r="I7" s="49"/>
+      <c r="I7" s="48"/>
       <c r="J7" s="19">
         <v>2000</v>
       </c>
       <c r="K7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="49"/>
+      <c r="L7" s="48"/>
     </row>
     <row r="8" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
@@ -1270,7 +1268,7 @@
       <c r="F8" s="33"/>
       <c r="G8" s="39"/>
       <c r="H8" s="36"/>
-      <c r="I8" s="49" t="s">
+      <c r="I8" s="48" t="s">
         <v>28</v>
       </c>
       <c r="J8" s="16">
@@ -1279,7 +1277,7 @@
       <c r="K8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="49"/>
+      <c r="L8" s="48"/>
     </row>
     <row r="9" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
@@ -1292,14 +1290,14 @@
       <c r="F9" s="3"/>
       <c r="G9" s="41"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="49"/>
+      <c r="I9" s="48"/>
       <c r="J9" s="19">
         <v>6500</v>
       </c>
       <c r="K9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="49"/>
+      <c r="L9" s="48"/>
     </row>
     <row r="10" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
@@ -1336,7 +1334,7 @@
       <c r="F11" s="33"/>
       <c r="G11" s="40"/>
       <c r="H11" s="33"/>
-      <c r="I11" s="49" t="s">
+      <c r="I11" s="48" t="s">
         <v>25</v>
       </c>
       <c r="J11" s="16">
@@ -1345,7 +1343,7 @@
       <c r="K11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="54" t="s">
+      <c r="L11" s="47" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1360,14 +1358,14 @@
       <c r="F12" s="3"/>
       <c r="G12" s="41"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="49"/>
+      <c r="I12" s="48"/>
       <c r="J12" s="14">
         <v>2300</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="49"/>
+      <c r="L12" s="48"/>
     </row>
     <row r="13" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
@@ -1380,14 +1378,14 @@
       <c r="F13" s="33"/>
       <c r="G13" s="39"/>
       <c r="H13" s="36"/>
-      <c r="I13" s="49"/>
+      <c r="I13" s="48"/>
       <c r="J13" s="14">
         <v>1800</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L13" s="49"/>
+      <c r="L13" s="48"/>
     </row>
     <row r="14" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
@@ -1400,14 +1398,14 @@
       <c r="F14" s="3"/>
       <c r="G14" s="41"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="49"/>
+      <c r="I14" s="48"/>
       <c r="J14" s="14">
         <v>2300</v>
       </c>
       <c r="K14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="L14" s="49"/>
+      <c r="L14" s="48"/>
     </row>
     <row r="15" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
@@ -1420,14 +1418,14 @@
       <c r="F15" s="33"/>
       <c r="G15" s="39"/>
       <c r="H15" s="36"/>
-      <c r="I15" s="49"/>
+      <c r="I15" s="48"/>
       <c r="J15" s="14">
         <v>3000</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L15" s="49"/>
+      <c r="L15" s="48"/>
     </row>
     <row r="16" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
@@ -1440,14 +1438,14 @@
       <c r="F16" s="3"/>
       <c r="G16" s="41"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="49"/>
+      <c r="I16" s="48"/>
       <c r="J16" s="15">
         <v>900</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="49"/>
+      <c r="L16" s="48"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
@@ -1471,7 +1469,7 @@
       <c r="K17" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="49"/>
+      <c r="L17" s="48"/>
     </row>
     <row r="18" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="28">
@@ -1484,7 +1482,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="41"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="55" t="s">
+      <c r="I18" s="49" t="s">
         <v>25</v>
       </c>
       <c r="J18" s="16">
@@ -1493,7 +1491,7 @@
       <c r="K18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L18" s="55" t="s">
+      <c r="L18" s="49" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1508,14 +1506,14 @@
       <c r="F19" s="33"/>
       <c r="G19" s="39"/>
       <c r="H19" s="36"/>
-      <c r="I19" s="55"/>
+      <c r="I19" s="49"/>
       <c r="J19" s="14">
         <v>2300</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L19" s="55"/>
+      <c r="L19" s="49"/>
     </row>
     <row r="20" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="28">
@@ -1528,14 +1526,14 @@
       <c r="F20" s="3"/>
       <c r="G20" s="41"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="55"/>
+      <c r="I20" s="49"/>
       <c r="J20" s="15">
         <v>1400</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="L20" s="55"/>
+      <c r="L20" s="49"/>
     </row>
     <row r="21" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
@@ -1548,7 +1546,7 @@
       <c r="F21" s="33"/>
       <c r="G21" s="39"/>
       <c r="H21" s="36"/>
-      <c r="I21" s="55"/>
+      <c r="I21" s="49"/>
       <c r="J21" s="9">
         <v>1100</v>
       </c>
@@ -1556,27 +1554,19 @@
         <v>24</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>52</v>
-      </c>
+      <c r="A23" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="L11:L17"/>
-    <mergeCell ref="L18:L20"/>
-    <mergeCell ref="I3:I7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I11:I16"/>
-    <mergeCell ref="I18:I21"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -1587,6 +1577,12 @@
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="L11:L17"/>
+    <mergeCell ref="L18:L20"/>
+    <mergeCell ref="I3:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I11:I16"/>
+    <mergeCell ref="I18:I21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated overview of materials
</commit_message>
<xml_diff>
--- a/docs/source/figures/Material_Database_Overview.xlsx
+++ b/docs/source/figures/Material_Database_Overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schacht\PycharmProjects\materialdatabase\docs\source\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899237BE-9BC8-4042-BB71-301E75171A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9762DB6-66B8-4A3C-847D-4BBC1EA3AE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E51A1F85-B08D-41FE-9B94-BB5FD5A5BD95}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E51A1F85-B08D-41FE-9B94-BB5FD5A5BD95}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -176,12 +176,6 @@
   </si>
   <si>
     <t>ML95S</t>
-  </si>
-  <si>
-    <t>µ</t>
-  </si>
-  <si>
-    <t>ε</t>
   </si>
   <si>
     <r>
@@ -224,6 +218,129 @@
   </si>
   <si>
     <t>*measurements from department Power Electronics and Electrical Drives at Paderborn University</t>
+  </si>
+  <si>
+    <r>
+      <t>µ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> T</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> B</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ε</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> T</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -274,13 +391,6 @@
     </font>
     <font>
       <b/>
-      <i/>
-      <sz val="16"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <vertAlign val="subscript"/>
       <sz val="16"/>
       <name val="Arial"/>
@@ -289,6 +399,12 @@
     <font>
       <b/>
       <i/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -567,7 +683,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -690,34 +806,22 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -730,6 +834,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1075,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83654C4-16D0-484A-BE01-4B99138EE44B}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,9 +1197,11 @@
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="7.140625" customWidth="1"/>
-    <col min="6" max="7" width="7" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.42578125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
     <col min="11" max="11" width="25.7109375" customWidth="1"/>
@@ -1096,62 +1211,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50" t="s">
+      <c r="G1" s="45"/>
+      <c r="H1" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="50"/>
-      <c r="H1" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" s="54" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="51" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" s="53"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="55"/>
+      <c r="E2" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="49"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="51"/>
     </row>
     <row r="3" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
@@ -1163,8 +1278,8 @@
       <c r="E3" s="22"/>
       <c r="F3" s="3"/>
       <c r="G3" s="38"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="48" t="s">
+      <c r="H3" s="43"/>
+      <c r="I3" s="47" t="s">
         <v>26</v>
       </c>
       <c r="J3" s="13">
@@ -1173,7 +1288,7 @@
       <c r="K3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="48" t="s">
+      <c r="L3" s="47" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1187,15 +1302,15 @@
       <c r="E4" s="35"/>
       <c r="F4" s="33"/>
       <c r="G4" s="39"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="48"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="47"/>
       <c r="J4" s="14">
         <v>2200</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="48"/>
+      <c r="L4" s="47"/>
     </row>
     <row r="5" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
@@ -1207,15 +1322,15 @@
       <c r="E5" s="31"/>
       <c r="F5" s="33"/>
       <c r="G5" s="40"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="48"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="47"/>
       <c r="J5" s="14">
         <v>1500</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="48"/>
+      <c r="L5" s="47"/>
     </row>
     <row r="6" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
@@ -1228,14 +1343,14 @@
       <c r="F6" s="33"/>
       <c r="G6" s="39"/>
       <c r="H6" s="33"/>
-      <c r="I6" s="48"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="14">
         <v>800</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="48"/>
+      <c r="L6" s="47"/>
     </row>
     <row r="7" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
@@ -1248,14 +1363,14 @@
       <c r="F7" s="33"/>
       <c r="G7" s="39"/>
       <c r="H7" s="36"/>
-      <c r="I7" s="48"/>
+      <c r="I7" s="47"/>
       <c r="J7" s="19">
         <v>2000</v>
       </c>
       <c r="K7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="48"/>
+      <c r="L7" s="47"/>
     </row>
     <row r="8" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
@@ -1268,7 +1383,7 @@
       <c r="F8" s="33"/>
       <c r="G8" s="39"/>
       <c r="H8" s="36"/>
-      <c r="I8" s="48" t="s">
+      <c r="I8" s="47" t="s">
         <v>28</v>
       </c>
       <c r="J8" s="16">
@@ -1277,7 +1392,7 @@
       <c r="K8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="48"/>
+      <c r="L8" s="47"/>
     </row>
     <row r="9" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
@@ -1290,14 +1405,14 @@
       <c r="F9" s="3"/>
       <c r="G9" s="41"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="48"/>
+      <c r="I9" s="47"/>
       <c r="J9" s="19">
         <v>6500</v>
       </c>
       <c r="K9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="48"/>
+      <c r="L9" s="47"/>
     </row>
     <row r="10" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
@@ -1334,7 +1449,7 @@
       <c r="F11" s="33"/>
       <c r="G11" s="40"/>
       <c r="H11" s="33"/>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="47" t="s">
         <v>25</v>
       </c>
       <c r="J11" s="16">
@@ -1343,7 +1458,7 @@
       <c r="K11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="47" t="s">
+      <c r="L11" s="52" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1358,14 +1473,14 @@
       <c r="F12" s="3"/>
       <c r="G12" s="41"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="48"/>
+      <c r="I12" s="47"/>
       <c r="J12" s="14">
         <v>2300</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="48"/>
+      <c r="L12" s="47"/>
     </row>
     <row r="13" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
@@ -1378,14 +1493,14 @@
       <c r="F13" s="33"/>
       <c r="G13" s="39"/>
       <c r="H13" s="36"/>
-      <c r="I13" s="48"/>
+      <c r="I13" s="47"/>
       <c r="J13" s="14">
         <v>1800</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L13" s="48"/>
+      <c r="L13" s="47"/>
     </row>
     <row r="14" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
@@ -1398,34 +1513,34 @@
       <c r="F14" s="3"/>
       <c r="G14" s="41"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="48"/>
+      <c r="I14" s="47"/>
       <c r="J14" s="14">
         <v>2300</v>
       </c>
       <c r="K14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="L14" s="48"/>
+      <c r="L14" s="47"/>
     </row>
     <row r="15" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="34"/>
+      <c r="B15" s="30"/>
       <c r="C15" s="35"/>
       <c r="D15" s="32"/>
       <c r="E15" s="35"/>
       <c r="F15" s="33"/>
       <c r="G15" s="39"/>
       <c r="H15" s="36"/>
-      <c r="I15" s="48"/>
+      <c r="I15" s="47"/>
       <c r="J15" s="14">
         <v>3000</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L15" s="48"/>
+      <c r="L15" s="47"/>
     </row>
     <row r="16" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
@@ -1438,14 +1553,14 @@
       <c r="F16" s="3"/>
       <c r="G16" s="41"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="48"/>
+      <c r="I16" s="47"/>
       <c r="J16" s="15">
         <v>900</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="48"/>
+      <c r="L16" s="47"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
@@ -1469,7 +1584,7 @@
       <c r="K17" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="48"/>
+      <c r="L17" s="47"/>
     </row>
     <row r="18" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="28">
@@ -1482,7 +1597,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="41"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="49" t="s">
+      <c r="I18" s="53" t="s">
         <v>25</v>
       </c>
       <c r="J18" s="16">
@@ -1491,7 +1606,7 @@
       <c r="K18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L18" s="49" t="s">
+      <c r="L18" s="53" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1506,14 +1621,14 @@
       <c r="F19" s="33"/>
       <c r="G19" s="39"/>
       <c r="H19" s="36"/>
-      <c r="I19" s="49"/>
+      <c r="I19" s="53"/>
       <c r="J19" s="14">
         <v>2300</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L19" s="49"/>
+      <c r="L19" s="53"/>
     </row>
     <row r="20" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="28">
@@ -1526,14 +1641,14 @@
       <c r="F20" s="3"/>
       <c r="G20" s="41"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="49"/>
+      <c r="I20" s="53"/>
       <c r="J20" s="15">
         <v>1400</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="L20" s="49"/>
+      <c r="L20" s="53"/>
     </row>
     <row r="21" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
@@ -1546,7 +1661,7 @@
       <c r="F21" s="33"/>
       <c r="G21" s="39"/>
       <c r="H21" s="36"/>
-      <c r="I21" s="49"/>
+      <c r="I21" s="53"/>
       <c r="J21" s="9">
         <v>1100</v>
       </c>
@@ -1554,12 +1669,12 @@
         <v>24</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1567,6 +1682,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="L11:L17"/>
+    <mergeCell ref="L18:L20"/>
+    <mergeCell ref="I3:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I11:I16"/>
+    <mergeCell ref="I18:I21"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -1577,12 +1698,6 @@
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="L11:L17"/>
-    <mergeCell ref="L18:L20"/>
-    <mergeCell ref="I3:I7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I11:I16"/>
-    <mergeCell ref="I18:I21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added datasheet data for 3F4, 3E6 and 3C90 added permittivity data for 3F4 and 3C90 updated overview of materials (ReadMe) added some additional Enumerations(Plotlabels)
</commit_message>
<xml_diff>
--- a/docs/source/figures/Material_Database_Overview.xlsx
+++ b/docs/source/figures/Material_Database_Overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schacht\PycharmProjects\materialdatabase\docs\source\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57ED0DC0-B4C2-48F4-AE1E-73E74BE4BB84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3254CD89-B224-4651-BE10-21AA5D1589E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E51A1F85-B08D-41FE-9B94-BB5FD5A5BD95}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E51A1F85-B08D-41FE-9B94-BB5FD5A5BD95}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -689,7 +689,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -824,19 +824,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -851,7 +848,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1197,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83654C4-16D0-484A-BE01-4B99138EE44B}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,43 +1223,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49" t="s">
+      <c r="E1" s="47"/>
+      <c r="F1" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="49"/>
+      <c r="G1" s="47"/>
       <c r="H1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="I1" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="J1" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="K1" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="L1" s="48" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="49"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="47"/>
       <c r="D2" s="45" t="s">
         <v>51</v>
       </c>
@@ -1272,10 +1275,10 @@
       <c r="H2" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="52"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="54"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="53"/>
     </row>
     <row r="3" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
@@ -1288,7 +1291,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="38"/>
       <c r="H3" s="43"/>
-      <c r="I3" s="47" t="s">
+      <c r="I3" s="49" t="s">
         <v>26</v>
       </c>
       <c r="J3" s="13">
@@ -1297,7 +1300,7 @@
       <c r="K3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="47" t="s">
+      <c r="L3" s="49" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1312,14 +1315,14 @@
       <c r="F4" s="33"/>
       <c r="G4" s="39"/>
       <c r="H4" s="44"/>
-      <c r="I4" s="47"/>
+      <c r="I4" s="49"/>
       <c r="J4" s="14">
         <v>2200</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="47"/>
+      <c r="L4" s="49"/>
     </row>
     <row r="5" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
@@ -1332,14 +1335,14 @@
       <c r="F5" s="33"/>
       <c r="G5" s="40"/>
       <c r="H5" s="44"/>
-      <c r="I5" s="47"/>
+      <c r="I5" s="49"/>
       <c r="J5" s="14">
         <v>1500</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="47"/>
+      <c r="L5" s="49"/>
     </row>
     <row r="6" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
@@ -1352,14 +1355,14 @@
       <c r="F6" s="33"/>
       <c r="G6" s="39"/>
       <c r="H6" s="33"/>
-      <c r="I6" s="47"/>
+      <c r="I6" s="49"/>
       <c r="J6" s="14">
         <v>800</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="47"/>
+      <c r="L6" s="49"/>
     </row>
     <row r="7" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
@@ -1372,14 +1375,14 @@
       <c r="F7" s="33"/>
       <c r="G7" s="39"/>
       <c r="H7" s="36"/>
-      <c r="I7" s="47"/>
+      <c r="I7" s="49"/>
       <c r="J7" s="19">
         <v>2000</v>
       </c>
       <c r="K7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="47"/>
+      <c r="L7" s="49"/>
     </row>
     <row r="8" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
@@ -1392,7 +1395,7 @@
       <c r="F8" s="33"/>
       <c r="G8" s="39"/>
       <c r="H8" s="36"/>
-      <c r="I8" s="47" t="s">
+      <c r="I8" s="49" t="s">
         <v>28</v>
       </c>
       <c r="J8" s="16">
@@ -1401,7 +1404,7 @@
       <c r="K8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="47"/>
+      <c r="L8" s="49"/>
     </row>
     <row r="9" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
@@ -1414,14 +1417,14 @@
       <c r="F9" s="3"/>
       <c r="G9" s="41"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="47"/>
+      <c r="I9" s="49"/>
       <c r="J9" s="19">
         <v>6500</v>
       </c>
       <c r="K9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="47"/>
+      <c r="L9" s="49"/>
     </row>
     <row r="10" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
@@ -1458,7 +1461,7 @@
       <c r="F11" s="33"/>
       <c r="G11" s="40"/>
       <c r="H11" s="33"/>
-      <c r="I11" s="47" t="s">
+      <c r="I11" s="49" t="s">
         <v>25</v>
       </c>
       <c r="J11" s="16">
@@ -1467,7 +1470,7 @@
       <c r="K11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="46" t="s">
+      <c r="L11" s="54" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1475,21 +1478,21 @@
       <c r="A12" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="21"/>
       <c r="C12" s="23"/>
       <c r="D12" s="5"/>
       <c r="E12" s="23"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="41"/>
+      <c r="G12" s="56"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="47"/>
+      <c r="I12" s="49"/>
       <c r="J12" s="14">
         <v>2300</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="47"/>
+      <c r="L12" s="49"/>
     </row>
     <row r="13" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
@@ -1502,14 +1505,14 @@
       <c r="F13" s="33"/>
       <c r="G13" s="39"/>
       <c r="H13" s="36"/>
-      <c r="I13" s="47"/>
+      <c r="I13" s="49"/>
       <c r="J13" s="14">
         <v>1800</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L13" s="47"/>
+      <c r="L13" s="49"/>
     </row>
     <row r="14" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
@@ -1522,54 +1525,54 @@
       <c r="F14" s="3"/>
       <c r="G14" s="41"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="47"/>
+      <c r="I14" s="49"/>
       <c r="J14" s="14">
         <v>2300</v>
       </c>
       <c r="K14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="L14" s="47"/>
+      <c r="L14" s="49"/>
     </row>
     <row r="15" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B15" s="30"/>
-      <c r="C15" s="35"/>
+      <c r="C15" s="31"/>
       <c r="D15" s="32"/>
       <c r="E15" s="35"/>
       <c r="F15" s="33"/>
-      <c r="G15" s="55"/>
+      <c r="G15" s="46"/>
       <c r="H15" s="36"/>
-      <c r="I15" s="47"/>
+      <c r="I15" s="49"/>
       <c r="J15" s="14">
         <v>3000</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L15" s="47"/>
+      <c r="L15" s="49"/>
     </row>
     <row r="16" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="23"/>
       <c r="D16" s="5"/>
       <c r="E16" s="23"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="41"/>
+      <c r="G16" s="56"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="47"/>
+      <c r="I16" s="49"/>
       <c r="J16" s="15">
         <v>900</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="47"/>
+      <c r="L16" s="49"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
@@ -1577,7 +1580,7 @@
       <c r="A17" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="34"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="35"/>
       <c r="D17" s="32"/>
       <c r="E17" s="35"/>
@@ -1593,7 +1596,7 @@
       <c r="K17" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="47"/>
+      <c r="L17" s="49"/>
     </row>
     <row r="18" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="28">
@@ -1606,7 +1609,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="41"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="48" t="s">
+      <c r="I18" s="55" t="s">
         <v>25</v>
       </c>
       <c r="J18" s="16">
@@ -1615,7 +1618,7 @@
       <c r="K18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L18" s="48" t="s">
+      <c r="L18" s="55" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1630,14 +1633,14 @@
       <c r="F19" s="33"/>
       <c r="G19" s="39"/>
       <c r="H19" s="36"/>
-      <c r="I19" s="48"/>
+      <c r="I19" s="55"/>
       <c r="J19" s="14">
         <v>2300</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L19" s="48"/>
+      <c r="L19" s="55"/>
     </row>
     <row r="20" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="28">
@@ -1650,14 +1653,14 @@
       <c r="F20" s="3"/>
       <c r="G20" s="41"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="48"/>
+      <c r="I20" s="55"/>
       <c r="J20" s="15">
         <v>1400</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="L20" s="48"/>
+      <c r="L20" s="55"/>
     </row>
     <row r="21" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
@@ -1670,7 +1673,7 @@
       <c r="F21" s="33"/>
       <c r="G21" s="39"/>
       <c r="H21" s="36"/>
-      <c r="I21" s="48"/>
+      <c r="I21" s="55"/>
       <c r="J21" s="9">
         <v>1100</v>
       </c>
@@ -1691,6 +1694,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="L11:L17"/>
+    <mergeCell ref="L18:L20"/>
+    <mergeCell ref="I3:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I11:I16"/>
+    <mergeCell ref="I18:I21"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -1701,12 +1710,6 @@
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="L11:L17"/>
-    <mergeCell ref="L18:L20"/>
-    <mergeCell ref="I3:I7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I11:I16"/>
-    <mergeCell ref="I18:I21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added datasheet values for 3C92 and 3C94 added permeability_data for 3C90, 3C92, 3C94 and 3F4
</commit_message>
<xml_diff>
--- a/docs/source/figures/Material_Database_Overview.xlsx
+++ b/docs/source/figures/Material_Database_Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schacht\PycharmProjects\materialdatabase\docs\source\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3254CD89-B224-4651-BE10-21AA5D1589E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8006910A-02D6-41DB-BB27-E56805D78411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E51A1F85-B08D-41FE-9B94-BB5FD5A5BD95}"/>
   </bookViews>
@@ -689,7 +689,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -827,13 +827,22 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -848,13 +857,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1201,7 +1204,7 @@
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,43 +1226,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47" t="s">
+      <c r="E1" s="51"/>
+      <c r="F1" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="47"/>
+      <c r="G1" s="51"/>
       <c r="H1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="J1" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="48" t="s">
+      <c r="L1" s="52" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="47"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="51"/>
       <c r="D2" s="45" t="s">
         <v>51</v>
       </c>
@@ -1275,10 +1278,10 @@
       <c r="H2" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="51"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="53"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="56"/>
     </row>
     <row r="3" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
@@ -1470,7 +1473,7 @@
       <c r="K11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="54" t="s">
+      <c r="L11" s="48" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1479,11 +1482,11 @@
         <v>39</v>
       </c>
       <c r="B12" s="21"/>
-      <c r="C12" s="23"/>
+      <c r="C12" s="57"/>
       <c r="D12" s="5"/>
       <c r="E12" s="23"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="56"/>
+      <c r="G12" s="47"/>
       <c r="H12" s="2"/>
       <c r="I12" s="49"/>
       <c r="J12" s="14">
@@ -1498,8 +1501,8 @@
       <c r="A13" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="35"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="32"/>
       <c r="E13" s="35"/>
       <c r="F13" s="33"/>
@@ -1518,8 +1521,8 @@
       <c r="A14" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="23"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="57"/>
       <c r="D14" s="5"/>
       <c r="E14" s="23"/>
       <c r="F14" s="3"/>
@@ -1559,11 +1562,11 @@
         <v>43</v>
       </c>
       <c r="B16" s="21"/>
-      <c r="C16" s="23"/>
+      <c r="C16" s="57"/>
       <c r="D16" s="5"/>
       <c r="E16" s="23"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="56"/>
+      <c r="G16" s="47"/>
       <c r="H16" s="2"/>
       <c r="I16" s="49"/>
       <c r="J16" s="15">
@@ -1609,7 +1612,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="41"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="55" t="s">
+      <c r="I18" s="50" t="s">
         <v>25</v>
       </c>
       <c r="J18" s="16">
@@ -1618,7 +1621,7 @@
       <c r="K18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L18" s="55" t="s">
+      <c r="L18" s="50" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1633,14 +1636,14 @@
       <c r="F19" s="33"/>
       <c r="G19" s="39"/>
       <c r="H19" s="36"/>
-      <c r="I19" s="55"/>
+      <c r="I19" s="50"/>
       <c r="J19" s="14">
         <v>2300</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L19" s="55"/>
+      <c r="L19" s="50"/>
     </row>
     <row r="20" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="28">
@@ -1653,14 +1656,14 @@
       <c r="F20" s="3"/>
       <c r="G20" s="41"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="55"/>
+      <c r="I20" s="50"/>
       <c r="J20" s="15">
         <v>1400</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="L20" s="55"/>
+      <c r="L20" s="50"/>
     </row>
     <row r="21" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
@@ -1673,7 +1676,7 @@
       <c r="F21" s="33"/>
       <c r="G21" s="39"/>
       <c r="H21" s="36"/>
-      <c r="I21" s="55"/>
+      <c r="I21" s="50"/>
       <c r="J21" s="9">
         <v>1100</v>
       </c>
@@ -1694,12 +1697,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="L11:L17"/>
-    <mergeCell ref="L18:L20"/>
-    <mergeCell ref="I3:I7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I11:I16"/>
-    <mergeCell ref="I18:I21"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -1710,6 +1707,12 @@
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="L11:L17"/>
+    <mergeCell ref="L18:L20"/>
+    <mergeCell ref="I3:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I11:I16"/>
+    <mergeCell ref="I18:I21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added datasheet values for 77, 78, 79, ML95S, 3F46, N27, N30 and T37
</commit_message>
<xml_diff>
--- a/docs/source/figures/Material_Database_Overview.xlsx
+++ b/docs/source/figures/Material_Database_Overview.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schacht\PycharmProjects\materialdatabase\docs\source\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8006910A-02D6-41DB-BB27-E56805D78411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3494255E-2491-4F5B-B00A-B7064EC6E333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E51A1F85-B08D-41FE-9B94-BB5FD5A5BD95}"/>
   </bookViews>
@@ -689,7 +689,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -788,9 +788,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -828,6 +825,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -855,9 +855,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1204,7 +1201,7 @@
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,7 +1240,7 @@
         <v>49</v>
       </c>
       <c r="G1" s="51"/>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="41" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="53" t="s">
@@ -1263,19 +1260,19 @@
       <c r="A2" s="52"/>
       <c r="B2" s="52"/>
       <c r="C2" s="51"/>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="45" t="s">
+      <c r="G2" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="45" t="s">
+      <c r="H2" s="44" t="s">
         <v>51</v>
       </c>
       <c r="I2" s="54"/>
@@ -1292,8 +1289,8 @@
       <c r="D3" s="21"/>
       <c r="E3" s="22"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="43"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="42"/>
       <c r="I3" s="49" t="s">
         <v>26</v>
       </c>
@@ -1313,11 +1310,11 @@
       </c>
       <c r="B4" s="30"/>
       <c r="C4" s="31"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="35"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="34"/>
       <c r="F4" s="33"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="44"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="43"/>
       <c r="I4" s="49"/>
       <c r="J4" s="14">
         <v>2200</v>
@@ -1333,11 +1330,11 @@
       </c>
       <c r="B5" s="30"/>
       <c r="C5" s="31"/>
-      <c r="D5" s="37"/>
+      <c r="D5" s="36"/>
       <c r="E5" s="31"/>
       <c r="F5" s="33"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="44"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="43"/>
       <c r="I5" s="49"/>
       <c r="J5" s="14">
         <v>1500</v>
@@ -1353,10 +1350,10 @@
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="31"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="35"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="34"/>
       <c r="F6" s="33"/>
-      <c r="G6" s="39"/>
+      <c r="G6" s="38"/>
       <c r="H6" s="33"/>
       <c r="I6" s="49"/>
       <c r="J6" s="14">
@@ -1371,13 +1368,13 @@
       <c r="A7" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="35"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="32"/>
-      <c r="E7" s="35"/>
+      <c r="E7" s="34"/>
       <c r="F7" s="33"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="36"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="35"/>
       <c r="I7" s="49"/>
       <c r="J7" s="19">
         <v>2000</v>
@@ -1391,13 +1388,13 @@
       <c r="A8" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="35"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="32"/>
-      <c r="E8" s="35"/>
+      <c r="E8" s="34"/>
       <c r="F8" s="33"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="36"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="35"/>
       <c r="I8" s="49" t="s">
         <v>28</v>
       </c>
@@ -1413,12 +1410,12 @@
       <c r="A9" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="23"/>
       <c r="D9" s="5"/>
       <c r="E9" s="23"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="41"/>
+      <c r="G9" s="40"/>
       <c r="H9" s="2"/>
       <c r="I9" s="49"/>
       <c r="J9" s="19">
@@ -1436,9 +1433,9 @@
       <c r="B10" s="30"/>
       <c r="C10" s="31"/>
       <c r="D10" s="32"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="40"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="39"/>
       <c r="H10" s="33"/>
       <c r="I10" s="10" t="s">
         <v>25</v>
@@ -1457,12 +1454,12 @@
       <c r="A11" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="35"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="34"/>
       <c r="D11" s="32"/>
-      <c r="E11" s="35"/>
+      <c r="E11" s="34"/>
       <c r="F11" s="33"/>
-      <c r="G11" s="40"/>
+      <c r="G11" s="39"/>
       <c r="H11" s="33"/>
       <c r="I11" s="49" t="s">
         <v>25</v>
@@ -1482,11 +1479,11 @@
         <v>39</v>
       </c>
       <c r="B12" s="21"/>
-      <c r="C12" s="57"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="5"/>
       <c r="E12" s="23"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="47"/>
+      <c r="G12" s="46"/>
       <c r="H12" s="2"/>
       <c r="I12" s="49"/>
       <c r="J12" s="14">
@@ -1504,10 +1501,10 @@
       <c r="B13" s="30"/>
       <c r="C13" s="31"/>
       <c r="D13" s="32"/>
-      <c r="E13" s="35"/>
+      <c r="E13" s="34"/>
       <c r="F13" s="33"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="36"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="35"/>
       <c r="I13" s="49"/>
       <c r="J13" s="14">
         <v>1800</v>
@@ -1522,11 +1519,11 @@
         <v>41</v>
       </c>
       <c r="B14" s="21"/>
-      <c r="C14" s="57"/>
+      <c r="C14" s="47"/>
       <c r="D14" s="5"/>
       <c r="E14" s="23"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="41"/>
+      <c r="G14" s="40"/>
       <c r="H14" s="2"/>
       <c r="I14" s="49"/>
       <c r="J14" s="14">
@@ -1544,10 +1541,10 @@
       <c r="B15" s="30"/>
       <c r="C15" s="31"/>
       <c r="D15" s="32"/>
-      <c r="E15" s="35"/>
+      <c r="E15" s="34"/>
       <c r="F15" s="33"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="36"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="35"/>
       <c r="I15" s="49"/>
       <c r="J15" s="14">
         <v>3000</v>
@@ -1562,11 +1559,11 @@
         <v>43</v>
       </c>
       <c r="B16" s="21"/>
-      <c r="C16" s="57"/>
+      <c r="C16" s="47"/>
       <c r="D16" s="5"/>
       <c r="E16" s="23"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="47"/>
+      <c r="G16" s="46"/>
       <c r="H16" s="2"/>
       <c r="I16" s="49"/>
       <c r="J16" s="15">
@@ -1584,12 +1581,12 @@
         <v>44</v>
       </c>
       <c r="B17" s="30"/>
-      <c r="C17" s="35"/>
+      <c r="C17" s="34"/>
       <c r="D17" s="32"/>
-      <c r="E17" s="35"/>
+      <c r="E17" s="34"/>
       <c r="F17" s="33"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="36"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="35"/>
       <c r="I17" s="10" t="s">
         <v>29</v>
       </c>
@@ -1605,12 +1602,12 @@
       <c r="A18" s="28">
         <v>77</v>
       </c>
-      <c r="B18" s="5"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="23"/>
       <c r="D18" s="5"/>
       <c r="E18" s="23"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="41"/>
+      <c r="G18" s="40"/>
       <c r="H18" s="2"/>
       <c r="I18" s="50" t="s">
         <v>25</v>
@@ -1629,13 +1626,13 @@
       <c r="A19" s="27">
         <v>78</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="35"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="34"/>
       <c r="D19" s="32"/>
-      <c r="E19" s="35"/>
+      <c r="E19" s="34"/>
       <c r="F19" s="33"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="36"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="35"/>
       <c r="I19" s="50"/>
       <c r="J19" s="14">
         <v>2300</v>
@@ -1649,12 +1646,12 @@
       <c r="A20" s="28">
         <v>79</v>
       </c>
-      <c r="B20" s="5"/>
+      <c r="B20" s="21"/>
       <c r="C20" s="23"/>
       <c r="D20" s="5"/>
       <c r="E20" s="23"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="41"/>
+      <c r="G20" s="40"/>
       <c r="H20" s="2"/>
       <c r="I20" s="50"/>
       <c r="J20" s="15">
@@ -1669,13 +1666,13 @@
       <c r="A21" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="34"/>
       <c r="D21" s="32"/>
-      <c r="E21" s="35"/>
+      <c r="E21" s="34"/>
       <c r="F21" s="33"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="36"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="35"/>
       <c r="I21" s="50"/>
       <c r="J21" s="9">
         <v>1100</v>

</xml_diff>

<commit_message>
added permeability_data for 77, 78, 79, 3F46 and N27 added script write_permeability_data_from_datasheet_into_database.py  -> script writes the data of datasheet plots into the database
</commit_message>
<xml_diff>
--- a/docs/source/figures/Material_Database_Overview.xlsx
+++ b/docs/source/figures/Material_Database_Overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schacht\PycharmProjects\materialdatabase\docs\source\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3494255E-2491-4F5B-B00A-B7064EC6E333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E103785-25A1-4D20-8A9F-94B27BA6F1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E51A1F85-B08D-41FE-9B94-BB5FD5A5BD95}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E51A1F85-B08D-41FE-9B94-BB5FD5A5BD95}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1200,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83654C4-16D0-484A-BE01-4B99138EE44B}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1369,7 +1369,7 @@
         <v>34</v>
       </c>
       <c r="B7" s="30"/>
-      <c r="C7" s="34"/>
+      <c r="C7" s="31"/>
       <c r="D7" s="32"/>
       <c r="E7" s="34"/>
       <c r="F7" s="33"/>
@@ -1455,7 +1455,7 @@
         <v>38</v>
       </c>
       <c r="B11" s="30"/>
-      <c r="C11" s="34"/>
+      <c r="C11" s="31"/>
       <c r="D11" s="32"/>
       <c r="E11" s="34"/>
       <c r="F11" s="33"/>
@@ -1603,7 +1603,7 @@
         <v>77</v>
       </c>
       <c r="B18" s="21"/>
-      <c r="C18" s="23"/>
+      <c r="C18" s="47"/>
       <c r="D18" s="5"/>
       <c r="E18" s="23"/>
       <c r="F18" s="3"/>
@@ -1627,7 +1627,7 @@
         <v>78</v>
       </c>
       <c r="B19" s="30"/>
-      <c r="C19" s="34"/>
+      <c r="C19" s="31"/>
       <c r="D19" s="32"/>
       <c r="E19" s="34"/>
       <c r="F19" s="33"/>
@@ -1647,7 +1647,7 @@
         <v>79</v>
       </c>
       <c r="B20" s="21"/>
-      <c r="C20" s="23"/>
+      <c r="C20" s="47"/>
       <c r="D20" s="5"/>
       <c r="E20" s="23"/>
       <c r="F20" s="3"/>

</xml_diff>

<commit_message>
updated functions in material_data_base_functions.py
</commit_message>
<xml_diff>
--- a/docs/source/figures/Material_Database_Overview.xlsx
+++ b/docs/source/figures/Material_Database_Overview.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schacht\PycharmProjects\materialdatabase\docs\source\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E103785-25A1-4D20-8A9F-94B27BA6F1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED6B2D2-87D4-4155-8787-B3073EBC9C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E51A1F85-B08D-41FE-9B94-BB5FD5A5BD95}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>Material</t>
   </si>
@@ -340,6 +340,107 @@
         <family val="2"/>
       </rPr>
       <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Steinmetz
+Parameter</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">k, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="17"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>α</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="17"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>β</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, k</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>**</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>**</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> parameter of IGSE</t>
     </r>
   </si>
 </sst>
@@ -347,7 +448,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,8 +516,42 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="17"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,8 +570,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE60000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -685,11 +826,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -809,40 +1003,50 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -855,6 +1059,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -865,9 +1090,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE60000"/>
       <color rgb="FFDA1010"/>
       <color rgb="FF9A0000"/>
-      <color rgb="FFE60000"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1198,10 +1423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83654C4-16D0-484A-BE01-4B99138EE44B}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,509 +1438,555 @@
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="25.7109375" customWidth="1"/>
-    <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.85546875" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="25.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.85546875" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:13" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51" t="s">
+      <c r="E1" s="62"/>
+      <c r="F1" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="51"/>
-      <c r="H1" s="41" t="s">
+      <c r="G1" s="65"/>
+      <c r="H1" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="J1" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="K1" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="55" t="s">
+      <c r="L1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="M1" s="55" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="44" t="s">
+    <row r="2" spans="1:13" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="60"/>
+    </row>
+    <row r="3" spans="1:13" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="55"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E3" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F3" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G3" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H3" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="54"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="56"/>
-    </row>
-    <row r="3" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+      <c r="J3" s="58"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="60"/>
+    </row>
+    <row r="4" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="49" t="s">
+      <c r="B4" s="21"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="13">
+      <c r="K4" s="13">
         <v>3000</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="L4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="49" t="s">
+      <c r="M4" s="53" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+    <row r="5" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="25" t="s">
         <v>31</v>
-      </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="14">
-        <v>2200</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="49"/>
-    </row>
-    <row r="5" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
-        <v>32</v>
       </c>
       <c r="B5" s="30"/>
       <c r="C5" s="31"/>
       <c r="D5" s="36"/>
-      <c r="E5" s="31"/>
+      <c r="E5" s="34"/>
       <c r="F5" s="33"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="14">
-        <v>1500</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L5" s="49"/>
-    </row>
-    <row r="6" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
-        <v>33</v>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="14">
+        <v>2200</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="53"/>
+    </row>
+    <row r="6" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
+        <v>32</v>
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="31"/>
       <c r="D6" s="36"/>
-      <c r="E6" s="34"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="33"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="14">
-        <v>800</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L6" s="49"/>
-    </row>
-    <row r="7" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
-        <v>34</v>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="14">
+        <v>1500</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="53"/>
+    </row>
+    <row r="7" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="25" t="s">
+        <v>33</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
+      <c r="D7" s="36"/>
       <c r="E7" s="34"/>
       <c r="F7" s="33"/>
       <c r="G7" s="38"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="19">
-        <v>2000</v>
-      </c>
-      <c r="K7" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" s="49"/>
-    </row>
-    <row r="8" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
-        <v>35</v>
+      <c r="H7" s="38"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="14">
+        <v>800</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="53"/>
+    </row>
+    <row r="8" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
+        <v>34</v>
       </c>
       <c r="B8" s="30"/>
-      <c r="C8" s="34"/>
+      <c r="C8" s="31"/>
       <c r="D8" s="32"/>
       <c r="E8" s="34"/>
       <c r="F8" s="33"/>
       <c r="G8" s="38"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="49" t="s">
+      <c r="H8" s="38"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="19">
+        <v>2000</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" s="53"/>
+    </row>
+    <row r="9" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="16">
+      <c r="K9" s="16">
         <v>4300</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="L9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="49"/>
-    </row>
-    <row r="9" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26" t="s">
+      <c r="M9" s="53"/>
+    </row>
+    <row r="10" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="19">
+      <c r="B10" s="21"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="19">
         <v>6500</v>
       </c>
-      <c r="K9" s="20" t="s">
+      <c r="L10" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="49"/>
-    </row>
-    <row r="10" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="25" t="s">
+      <c r="M10" s="53"/>
+    </row>
+    <row r="11" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="25" t="s">
         <v>37</v>
-      </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="17">
-        <v>3500</v>
-      </c>
-      <c r="K10" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26" t="s">
-        <v>38</v>
       </c>
       <c r="B11" s="30"/>
       <c r="C11" s="31"/>
       <c r="D11" s="32"/>
       <c r="E11" s="34"/>
-      <c r="F11" s="33"/>
+      <c r="F11" s="35"/>
       <c r="G11" s="39"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="49" t="s">
+      <c r="H11" s="48"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="16">
+      <c r="K11" s="17">
+        <v>3500</v>
+      </c>
+      <c r="L11" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="30"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="16">
         <v>750</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="L12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="48" t="s">
+      <c r="M12" s="52" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+    <row r="13" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="14">
+      <c r="B13" s="21"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="14">
         <v>2300</v>
       </c>
-      <c r="K12" s="6" t="s">
+      <c r="L13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="49"/>
-    </row>
-    <row r="13" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26" t="s">
+      <c r="M13" s="53"/>
+    </row>
+    <row r="14" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="14">
+      <c r="B14" s="30"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="14">
         <v>1800</v>
       </c>
-      <c r="K13" s="6" t="s">
+      <c r="L14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L13" s="49"/>
-    </row>
-    <row r="14" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="25" t="s">
+      <c r="M14" s="53"/>
+    </row>
+    <row r="15" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="14">
+      <c r="B15" s="21"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="14">
         <v>2300</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="L15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="L14" s="49"/>
-    </row>
-    <row r="15" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
+      <c r="M15" s="53"/>
+    </row>
+    <row r="16" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="14">
+      <c r="B16" s="30"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="14">
         <v>3000</v>
       </c>
-      <c r="K15" s="6" t="s">
+      <c r="L16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L15" s="49"/>
-    </row>
-    <row r="16" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="25" t="s">
+      <c r="M16" s="53"/>
+    </row>
+    <row r="17" spans="1:17" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="15">
+      <c r="B17" s="21"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="15">
         <v>900</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="L17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="49"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-    </row>
-    <row r="17" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27" t="s">
+      <c r="M17" s="53"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" spans="1:17" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="10" t="s">
+      <c r="B18" s="30"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J17" s="9">
+      <c r="K18" s="9">
         <v>10000</v>
       </c>
-      <c r="K17" s="11" t="s">
+      <c r="L18" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="49"/>
-    </row>
-    <row r="18" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="28">
+      <c r="M18" s="53"/>
+    </row>
+    <row r="19" spans="1:17" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="28">
         <v>77</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="50" t="s">
+      <c r="B19" s="21"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="J18" s="16">
+      <c r="K19" s="16">
         <v>2000</v>
       </c>
-      <c r="K18" s="7" t="s">
+      <c r="L19" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L18" s="50" t="s">
+      <c r="M19" s="54" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="27">
+    <row r="20" spans="1:17" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="27">
         <v>78</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="14">
+      <c r="B20" s="30"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="14">
         <v>2300</v>
       </c>
-      <c r="K19" s="6" t="s">
+      <c r="L20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L19" s="50"/>
-    </row>
-    <row r="20" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="28">
+      <c r="M20" s="54"/>
+    </row>
+    <row r="21" spans="1:17" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="28">
         <v>79</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="15">
+      <c r="B21" s="21"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="15">
         <v>1400</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="L21" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="L20" s="50"/>
-    </row>
-    <row r="21" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="29" t="s">
+      <c r="M21" s="54"/>
+    </row>
+    <row r="22" spans="1:17" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="9">
+      <c r="B22" s="30"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="9">
         <v>1100</v>
       </c>
-      <c r="K21" s="12" t="s">
+      <c r="L22" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="L21" s="10" t="s">
+      <c r="M22" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+    <row r="23" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
+      <c r="H23" s="46"/>
+    </row>
+    <row r="24" spans="1:17" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="L3:L9"/>
+  <mergeCells count="18">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="M4:M10"/>
+    <mergeCell ref="J1:J3"/>
+    <mergeCell ref="K1:K3"/>
+    <mergeCell ref="L1:L3"/>
+    <mergeCell ref="M1:M3"/>
+    <mergeCell ref="D1:E2"/>
+    <mergeCell ref="F1:G2"/>
+    <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="L11:L17"/>
-    <mergeCell ref="L18:L20"/>
-    <mergeCell ref="I3:I7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I11:I16"/>
-    <mergeCell ref="I18:I21"/>
+    <mergeCell ref="M12:M18"/>
+    <mergeCell ref="M19:M21"/>
+    <mergeCell ref="J4:J8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J12:J17"/>
+    <mergeCell ref="J19:J22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A17" numberStoredAsText="1"/>
+    <ignoredError sqref="A18" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- added permittivity data for materials N27, N30, 3C92 and 3C94  - updated permittivity data for material 3F46, 3F4, 3C90, 3C95 and N49 (added more frequency points)  - updated README file to explain different data types in table
</commit_message>
<xml_diff>
--- a/docs/source/figures/Material_Database_Overview.xlsx
+++ b/docs/source/figures/Material_Database_Overview.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schacht\PycharmProjects\materialdatabase\docs\source\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E103785-25A1-4D20-8A9F-94B27BA6F1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEE8EA5-4A8D-4966-9600-61C18CE0B34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E51A1F85-B08D-41FE-9B94-BB5FD5A5BD95}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
   <si>
     <t>Material</t>
   </si>
@@ -208,16 +208,7 @@
     </r>
   </si>
   <si>
-    <t>LEA_LK*</t>
-  </si>
-  <si>
     <t>Proterial</t>
-  </si>
-  <si>
-    <t>LEA_MTB*</t>
-  </si>
-  <si>
-    <t>*measurements from department Power Electronics and Electrical Drives at Paderborn University</t>
   </si>
   <si>
     <r>
@@ -341,6 +332,12 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>LEA_MTB</t>
+  </si>
+  <si>
+    <t>LEA_LK</t>
   </si>
 </sst>
 </file>
@@ -689,7 +686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -829,6 +826,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1200,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83654C4-16D0-484A-BE01-4B99138EE44B}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,62 +1223,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="51"/>
+      <c r="D1" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="52"/>
       <c r="H1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="I1" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="55" t="s">
+      <c r="K1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="53" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="51"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="44" t="s">
+        <v>48</v>
+      </c>
       <c r="D2" s="44" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F2" s="44" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G2" s="44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H2" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="I2" s="54"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="56"/>
+        <v>48</v>
+      </c>
+      <c r="I2" s="55"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="57"/>
     </row>
     <row r="3" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
@@ -1291,7 +1293,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="37"/>
       <c r="H3" s="42"/>
-      <c r="I3" s="49" t="s">
+      <c r="I3" s="50" t="s">
         <v>26</v>
       </c>
       <c r="J3" s="13">
@@ -1300,7 +1302,7 @@
       <c r="K3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="49" t="s">
+      <c r="L3" s="50" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1315,14 +1317,14 @@
       <c r="F4" s="33"/>
       <c r="G4" s="38"/>
       <c r="H4" s="43"/>
-      <c r="I4" s="49"/>
+      <c r="I4" s="50"/>
       <c r="J4" s="14">
         <v>2200</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="49"/>
+      <c r="L4" s="50"/>
     </row>
     <row r="5" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
@@ -1335,14 +1337,14 @@
       <c r="F5" s="33"/>
       <c r="G5" s="39"/>
       <c r="H5" s="43"/>
-      <c r="I5" s="49"/>
+      <c r="I5" s="50"/>
       <c r="J5" s="14">
         <v>1500</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="49"/>
+      <c r="L5" s="50"/>
     </row>
     <row r="6" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
@@ -1355,14 +1357,14 @@
       <c r="F6" s="33"/>
       <c r="G6" s="38"/>
       <c r="H6" s="33"/>
-      <c r="I6" s="49"/>
+      <c r="I6" s="50"/>
       <c r="J6" s="14">
         <v>800</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="49"/>
+      <c r="L6" s="50"/>
     </row>
     <row r="7" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
@@ -1373,16 +1375,16 @@
       <c r="D7" s="32"/>
       <c r="E7" s="34"/>
       <c r="F7" s="33"/>
-      <c r="G7" s="38"/>
+      <c r="G7" s="39"/>
       <c r="H7" s="35"/>
-      <c r="I7" s="49"/>
+      <c r="I7" s="50"/>
       <c r="J7" s="19">
         <v>2000</v>
       </c>
       <c r="K7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="49"/>
+      <c r="L7" s="50"/>
     </row>
     <row r="8" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
@@ -1393,9 +1395,9 @@
       <c r="D8" s="32"/>
       <c r="E8" s="34"/>
       <c r="F8" s="33"/>
-      <c r="G8" s="38"/>
+      <c r="G8" s="39"/>
       <c r="H8" s="35"/>
-      <c r="I8" s="49" t="s">
+      <c r="I8" s="50" t="s">
         <v>28</v>
       </c>
       <c r="J8" s="16">
@@ -1404,7 +1406,7 @@
       <c r="K8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="49"/>
+      <c r="L8" s="50"/>
     </row>
     <row r="9" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
@@ -1417,14 +1419,14 @@
       <c r="F9" s="3"/>
       <c r="G9" s="40"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="49"/>
+      <c r="I9" s="50"/>
       <c r="J9" s="19">
         <v>6500</v>
       </c>
       <c r="K9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="49"/>
+      <c r="L9" s="50"/>
     </row>
     <row r="10" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
@@ -1461,7 +1463,7 @@
       <c r="F11" s="33"/>
       <c r="G11" s="39"/>
       <c r="H11" s="33"/>
-      <c r="I11" s="49" t="s">
+      <c r="I11" s="50" t="s">
         <v>25</v>
       </c>
       <c r="J11" s="16">
@@ -1470,7 +1472,7 @@
       <c r="K11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="48" t="s">
+      <c r="L11" s="49" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1485,14 +1487,14 @@
       <c r="F12" s="3"/>
       <c r="G12" s="46"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="49"/>
+      <c r="I12" s="50"/>
       <c r="J12" s="14">
         <v>2300</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="49"/>
+      <c r="L12" s="50"/>
     </row>
     <row r="13" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
@@ -1503,16 +1505,16 @@
       <c r="D13" s="32"/>
       <c r="E13" s="34"/>
       <c r="F13" s="33"/>
-      <c r="G13" s="38"/>
+      <c r="G13" s="39"/>
       <c r="H13" s="35"/>
-      <c r="I13" s="49"/>
+      <c r="I13" s="50"/>
       <c r="J13" s="14">
         <v>1800</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L13" s="49"/>
+      <c r="L13" s="50"/>
     </row>
     <row r="14" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
@@ -1523,16 +1525,16 @@
       <c r="D14" s="5"/>
       <c r="E14" s="23"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="40"/>
+      <c r="G14" s="46"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="49"/>
+      <c r="I14" s="50"/>
       <c r="J14" s="14">
         <v>2300</v>
       </c>
       <c r="K14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="L14" s="49"/>
+      <c r="L14" s="50"/>
     </row>
     <row r="15" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
@@ -1545,14 +1547,14 @@
       <c r="F15" s="33"/>
       <c r="G15" s="45"/>
       <c r="H15" s="35"/>
-      <c r="I15" s="49"/>
+      <c r="I15" s="50"/>
       <c r="J15" s="14">
         <v>3000</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L15" s="49"/>
+      <c r="L15" s="50"/>
     </row>
     <row r="16" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
@@ -1565,14 +1567,14 @@
       <c r="F16" s="3"/>
       <c r="G16" s="46"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="49"/>
+      <c r="I16" s="50"/>
       <c r="J16" s="15">
         <v>900</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="49"/>
+      <c r="L16" s="50"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
@@ -1596,7 +1598,7 @@
       <c r="K17" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="49"/>
+      <c r="L17" s="50"/>
     </row>
     <row r="18" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="28">
@@ -1609,7 +1611,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="40"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="50" t="s">
+      <c r="I18" s="51" t="s">
         <v>25</v>
       </c>
       <c r="J18" s="16">
@@ -1618,7 +1620,7 @@
       <c r="K18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L18" s="50" t="s">
+      <c r="L18" s="51" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1633,14 +1635,14 @@
       <c r="F19" s="33"/>
       <c r="G19" s="38"/>
       <c r="H19" s="35"/>
-      <c r="I19" s="50"/>
+      <c r="I19" s="51"/>
       <c r="J19" s="14">
         <v>2300</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L19" s="50"/>
+      <c r="L19" s="51"/>
     </row>
     <row r="20" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="28">
@@ -1653,14 +1655,14 @@
       <c r="F20" s="3"/>
       <c r="G20" s="40"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="50"/>
+      <c r="I20" s="51"/>
       <c r="J20" s="15">
         <v>1400</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="L20" s="50"/>
+      <c r="L20" s="51"/>
     </row>
     <row r="21" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
@@ -1673,7 +1675,7 @@
       <c r="F21" s="33"/>
       <c r="G21" s="38"/>
       <c r="H21" s="35"/>
-      <c r="I21" s="50"/>
+      <c r="I21" s="51"/>
       <c r="J21" s="9">
         <v>1100</v>
       </c>
@@ -1681,23 +1683,20 @@
         <v>24</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="A22" s="4"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="15">
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
     <mergeCell ref="L3:L9"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>

</xml_diff>

<commit_message>
updated material_data_base.json and Material_Database_Overview.xlsx to main (because of merge conflict)
</commit_message>
<xml_diff>
--- a/docs/source/figures/Material_Database_Overview.xlsx
+++ b/docs/source/figures/Material_Database_Overview.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schacht\PycharmProjects\materialdatabase\docs\source\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED6B2D2-87D4-4155-8787-B3073EBC9C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEE8EA5-4A8D-4966-9600-61C18CE0B34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E51A1F85-B08D-41FE-9B94-BB5FD5A5BD95}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
   <si>
     <t>Material</t>
   </si>
@@ -208,16 +208,7 @@
     </r>
   </si>
   <si>
-    <t>LEA_LK*</t>
-  </si>
-  <si>
     <t>Proterial</t>
-  </si>
-  <si>
-    <t>LEA_MTB*</t>
-  </si>
-  <si>
-    <t>*measurements from department Power Electronics and Electrical Drives at Paderborn University</t>
   </si>
   <si>
     <r>
@@ -343,112 +334,17 @@
     </r>
   </si>
   <si>
-    <t>Steinmetz
-Parameter</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">k, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="17"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>α</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="17"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>β</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, k</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>i</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>**</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>**</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>k</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> parameter of IGSE</t>
-    </r>
+    <t>LEA_MTB</t>
+  </si>
+  <si>
+    <t>LEA_LK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -516,42 +412,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <vertAlign val="subscript"/>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="17"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <vertAlign val="subscript"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -570,14 +432,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE60000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="25">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -826,64 +682,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1003,6 +806,15 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1015,24 +827,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1043,10 +839,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1059,27 +855,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1090,9 +865,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFE60000"/>
       <color rgb="FFDA1010"/>
       <color rgb="FF9A0000"/>
+      <color rgb="FFE60000"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1423,10 +1198,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83654C4-16D0-484A-BE01-4B99138EE44B}">
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,555 +1213,508 @@
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.42578125" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="25.7109375" customWidth="1"/>
-    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.85546875" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.85546875" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:16" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="62"/>
-      <c r="F1" s="61" t="s">
+      <c r="D1" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="52"/>
+      <c r="H1" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="65"/>
-      <c r="H1" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="62" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="56" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="59" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="55" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="58"/>
+      <c r="F2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="55"/>
+      <c r="J2" s="52"/>
       <c r="K2" s="56"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="60"/>
-    </row>
-    <row r="3" spans="1:13" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="58"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="60"/>
-    </row>
-    <row r="4" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
+      <c r="L2" s="57"/>
+    </row>
+    <row r="3" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="53" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="13">
+      <c r="J3" s="13">
         <v>3000</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="53" t="s">
+      <c r="L3" s="50" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+    <row r="4" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
         <v>31</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="14">
+        <v>2200</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="50"/>
+    </row>
+    <row r="5" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
+        <v>32</v>
       </c>
       <c r="B5" s="30"/>
       <c r="C5" s="31"/>
       <c r="D5" s="36"/>
-      <c r="E5" s="34"/>
+      <c r="E5" s="31"/>
       <c r="F5" s="33"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="14">
-        <v>2200</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="53"/>
-    </row>
-    <row r="6" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
-        <v>32</v>
+      <c r="G5" s="39"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="14">
+        <v>1500</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="50"/>
+    </row>
+    <row r="6" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25" t="s">
+        <v>33</v>
       </c>
       <c r="B6" s="30"/>
       <c r="C6" s="31"/>
       <c r="D6" s="36"/>
-      <c r="E6" s="31"/>
+      <c r="E6" s="34"/>
       <c r="F6" s="33"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="14">
-        <v>1500</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M6" s="53"/>
-    </row>
-    <row r="7" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
-        <v>33</v>
+      <c r="G6" s="38"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="14">
+        <v>800</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="50"/>
+    </row>
+    <row r="7" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
+        <v>34</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="31"/>
-      <c r="D7" s="36"/>
+      <c r="D7" s="32"/>
       <c r="E7" s="34"/>
       <c r="F7" s="33"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="14">
-        <v>800</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="M7" s="53"/>
-    </row>
-    <row r="8" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
-        <v>34</v>
+      <c r="G7" s="39"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="19">
+        <v>2000</v>
+      </c>
+      <c r="K7" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="50"/>
+    </row>
+    <row r="8" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="B8" s="30"/>
-      <c r="C8" s="31"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="32"/>
       <c r="E8" s="34"/>
       <c r="F8" s="33"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="19">
-        <v>2000</v>
-      </c>
-      <c r="L8" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="M8" s="53"/>
-    </row>
-    <row r="9" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="53" t="s">
+      <c r="G8" s="39"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="K9" s="16">
+      <c r="J8" s="16">
         <v>4300</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="K8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="M9" s="53"/>
-    </row>
-    <row r="10" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
+      <c r="L8" s="50"/>
+    </row>
+    <row r="9" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="19">
+      <c r="B9" s="21"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="19">
         <v>6500</v>
       </c>
-      <c r="L10" s="20" t="s">
+      <c r="K9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="M10" s="53"/>
-    </row>
-    <row r="11" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="25" t="s">
+      <c r="L9" s="50"/>
+    </row>
+    <row r="10" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="25" t="s">
         <v>37</v>
+      </c>
+      <c r="B10" s="30"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="17">
+        <v>3500</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="26" t="s">
+        <v>38</v>
       </c>
       <c r="B11" s="30"/>
       <c r="C11" s="31"/>
       <c r="D11" s="32"/>
       <c r="E11" s="34"/>
-      <c r="F11" s="35"/>
+      <c r="F11" s="33"/>
       <c r="G11" s="39"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="10" t="s">
+      <c r="H11" s="33"/>
+      <c r="I11" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="17">
-        <v>3500</v>
-      </c>
-      <c r="L11" s="18" t="s">
+      <c r="J11" s="16">
+        <v>750</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="14">
+        <v>2300</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" s="50"/>
+    </row>
+    <row r="13" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="30"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="14">
+        <v>1800</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="50"/>
+    </row>
+    <row r="14" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="14">
+        <v>2300</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="50"/>
+    </row>
+    <row r="15" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="14">
+        <v>3000</v>
+      </c>
+      <c r="K15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="M11" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="53" t="s">
+      <c r="L15" s="50"/>
+    </row>
+    <row r="16" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="15">
+        <v>900</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="50"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="30"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" s="9">
+        <v>10000</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="50"/>
+    </row>
+    <row r="18" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="28">
+        <v>77</v>
+      </c>
+      <c r="B18" s="21"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="K12" s="16">
-        <v>750</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M12" s="52" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="14">
+      <c r="J18" s="16">
+        <v>2000</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="27">
+        <v>78</v>
+      </c>
+      <c r="B19" s="30"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="14">
         <v>2300</v>
       </c>
-      <c r="L13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="M13" s="53"/>
-    </row>
-    <row r="14" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="14">
-        <v>1800</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="M14" s="53"/>
-    </row>
-    <row r="15" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="14">
-        <v>2300</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" s="53"/>
-    </row>
-    <row r="16" spans="1:13" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="14">
-        <v>3000</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="M16" s="53"/>
-    </row>
-    <row r="17" spans="1:17" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="15">
-        <v>900</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="M17" s="53"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-    </row>
-    <row r="18" spans="1:17" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="K18" s="9">
-        <v>10000</v>
-      </c>
-      <c r="L18" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="M18" s="53"/>
-    </row>
-    <row r="19" spans="1:17" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="28">
-        <v>77</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="54" t="s">
-        <v>25</v>
-      </c>
-      <c r="K19" s="16">
-        <v>2000</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M19" s="54" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="27">
-        <v>78</v>
-      </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="54"/>
-      <c r="K20" s="14">
-        <v>2300</v>
-      </c>
-      <c r="L20" s="6" t="s">
+      <c r="K19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M20" s="54"/>
-    </row>
-    <row r="21" spans="1:17" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28">
+      <c r="L19" s="51"/>
+    </row>
+    <row r="20" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="28">
         <v>79</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="15">
+      <c r="B20" s="21"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="15">
         <v>1400</v>
       </c>
-      <c r="L21" s="8" t="s">
+      <c r="K20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="M21" s="54"/>
-    </row>
-    <row r="22" spans="1:17" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="29" t="s">
+      <c r="L20" s="51"/>
+    </row>
+    <row r="21" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="9">
+      <c r="B21" s="30"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="9">
         <v>1100</v>
       </c>
-      <c r="L22" s="12" t="s">
+      <c r="K21" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="M22" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H23" s="46"/>
-    </row>
-    <row r="24" spans="1:17" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="L21" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="M4:M10"/>
-    <mergeCell ref="J1:J3"/>
-    <mergeCell ref="K1:K3"/>
-    <mergeCell ref="L1:L3"/>
-    <mergeCell ref="M1:M3"/>
-    <mergeCell ref="D1:E2"/>
-    <mergeCell ref="F1:G2"/>
-    <mergeCell ref="H1:H2"/>
+  <mergeCells count="15">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="L3:L9"/>
     <mergeCell ref="I1:I2"/>
-    <mergeCell ref="M12:M18"/>
-    <mergeCell ref="M19:M21"/>
-    <mergeCell ref="J4:J8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J12:J17"/>
-    <mergeCell ref="J19:J22"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="L11:L17"/>
+    <mergeCell ref="L18:L20"/>
+    <mergeCell ref="I3:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I11:I16"/>
+    <mergeCell ref="I18:I21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A18" numberStoredAsText="1"/>
+    <ignoredError sqref="A17" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated README and overview of material data in MDB
</commit_message>
<xml_diff>
--- a/docs/source/figures/Material_Database_Overview.xlsx
+++ b/docs/source/figures/Material_Database_Overview.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schacht\PycharmProjects\materialdatabase\docs\source\figures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Repositorys\materialdatabase\docs\source\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEE8EA5-4A8D-4966-9600-61C18CE0B34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D4E33C-F418-4CA9-BD9E-6D75B287A29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E51A1F85-B08D-41FE-9B94-BB5FD5A5BD95}"/>
   </bookViews>
@@ -27,16 +27,17 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
   <si>
     <t>Material</t>
   </si>
@@ -337,14 +338,14 @@
     <t>LEA_MTB</t>
   </si>
   <si>
-    <t>LEA_LK</t>
+    <t>TDK_MDT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,12 +407,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF92D050"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -433,7 +428,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -615,21 +610,6 @@
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -691,16 +671,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -737,22 +708,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -761,70 +729,31 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -836,13 +765,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -855,6 +784,57 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1198,67 +1178,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83654C4-16D0-484A-BE01-4B99138EE44B}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="25.7109375" customWidth="1"/>
-    <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.85546875" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.75" customWidth="1"/>
+    <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="3" max="3" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.375" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="25.75" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.875" customWidth="1"/>
+    <col min="13" max="13" width="16.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:15" ht="21" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52" t="s">
+      <c r="E1" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="41" t="s">
+      <c r="F1" s="34"/>
+      <c r="G1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="54" t="s">
+      <c r="H1" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="I1" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="56" t="s">
+      <c r="J1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="53" t="s">
+      <c r="K1" s="35" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53"/>
+    <row r="2" spans="1:15" ht="21" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
       <c r="C2" s="44" t="s">
         <v>48</v>
       </c>
@@ -1266,449 +1243,426 @@
         <v>48</v>
       </c>
       <c r="E2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="G2" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="55"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="57"/>
-    </row>
-    <row r="3" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+      <c r="H2" s="38"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="40"/>
+    </row>
+    <row r="3" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A3" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="50" t="s">
+      <c r="B3" s="48"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="13">
+      <c r="I3" s="10">
         <v>3000</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="J3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="50" t="s">
+      <c r="K3" s="36" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+    <row r="4" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A4" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="14">
+      <c r="B4" s="52"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="11">
         <v>2200</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="J4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="50"/>
-    </row>
-    <row r="5" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
+      <c r="K4" s="36"/>
+    </row>
+    <row r="5" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A5" s="22" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="14">
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="11">
         <v>1500</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="J5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="50"/>
-    </row>
-    <row r="6" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
+      <c r="K5" s="36"/>
+    </row>
+    <row r="6" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A6" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="14">
+      <c r="B6" s="52"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="11">
         <v>800</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="J6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="50"/>
-    </row>
-    <row r="7" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="K6" s="36"/>
+    </row>
+    <row r="7" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A7" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="19">
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="16">
         <v>2000</v>
       </c>
-      <c r="K7" s="20" t="s">
+      <c r="J7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="50"/>
-    </row>
-    <row r="8" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
+      <c r="K7" s="36"/>
+    </row>
+    <row r="8" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A8" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="50" t="s">
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="16">
+      <c r="I8" s="13">
         <v>4300</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="J8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="50"/>
-    </row>
-    <row r="9" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26" t="s">
+      <c r="K8" s="36"/>
+    </row>
+    <row r="9" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A9" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="19">
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="16">
         <v>6500</v>
       </c>
-      <c r="K9" s="20" t="s">
+      <c r="J9" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="50"/>
-    </row>
-    <row r="10" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="25" t="s">
+      <c r="K9" s="36"/>
+    </row>
+    <row r="10" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A10" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="10" t="s">
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="17">
+      <c r="I10" s="14">
         <v>3500</v>
       </c>
-      <c r="K10" s="18" t="s">
+      <c r="J10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="K10" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26" t="s">
+    <row r="11" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A11" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="50" t="s">
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="16">
+      <c r="I11" s="13">
         <v>750</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="J11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="49" t="s">
+      <c r="K11" s="41" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+    <row r="12" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A12" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="14">
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="11">
         <v>2300</v>
       </c>
-      <c r="K12" s="6" t="s">
+      <c r="J12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="50"/>
-    </row>
-    <row r="13" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26" t="s">
+      <c r="K12" s="36"/>
+    </row>
+    <row r="13" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A13" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="14">
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="11">
         <v>1800</v>
       </c>
-      <c r="K13" s="6" t="s">
+      <c r="J13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L13" s="50"/>
-    </row>
-    <row r="14" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="25" t="s">
+      <c r="K13" s="36"/>
+    </row>
+    <row r="14" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A14" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="14">
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="11">
         <v>2300</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="J14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L14" s="50"/>
-    </row>
-    <row r="15" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
+      <c r="K14" s="36"/>
+    </row>
+    <row r="15" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A15" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="14">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="11">
         <v>3000</v>
       </c>
-      <c r="K15" s="6" t="s">
+      <c r="J15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L15" s="50"/>
-    </row>
-    <row r="16" spans="1:16" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="25" t="s">
+      <c r="K15" s="36"/>
+    </row>
+    <row r="16" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A16" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="15">
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="12">
         <v>900</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="J16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="50"/>
+      <c r="K16" s="36"/>
+      <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-    </row>
-    <row r="17" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27" t="s">
+    </row>
+    <row r="17" spans="1:11" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A17" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="10" t="s">
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="J17" s="9">
+      <c r="I17" s="6">
         <v>10000</v>
       </c>
-      <c r="K17" s="11" t="s">
+      <c r="J17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="50"/>
-    </row>
-    <row r="18" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="28">
+      <c r="K17" s="36"/>
+    </row>
+    <row r="18" spans="1:11" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A18" s="57">
         <v>77</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="51" t="s">
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="J18" s="16">
+      <c r="I18" s="13">
         <v>2000</v>
       </c>
-      <c r="K18" s="7" t="s">
+      <c r="J18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L18" s="51" t="s">
+      <c r="K18" s="42" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="27">
+    <row r="19" spans="1:11" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A19" s="23">
         <v>78</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="14">
+      <c r="B19" s="52"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="11">
         <v>2300</v>
       </c>
-      <c r="K19" s="6" t="s">
+      <c r="J19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L19" s="51"/>
-    </row>
-    <row r="20" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="28">
+      <c r="K19" s="42"/>
+    </row>
+    <row r="20" spans="1:11" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A20" s="56">
         <v>79</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="15">
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="12">
         <v>1400</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="J20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L20" s="51"/>
-    </row>
-    <row r="21" spans="1:12" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="29" t="s">
+      <c r="K20" s="42"/>
+    </row>
+    <row r="21" spans="1:11" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A21" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="9">
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="6">
         <v>1100</v>
       </c>
-      <c r="K21" s="12" t="s">
+      <c r="J21" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="L21" s="10" t="s">
+      <c r="K21" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
+    <row r="22" spans="1:11" ht="15" thickTop="1">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="D1:E1"/>
+  <mergeCells count="14">
+    <mergeCell ref="K11:K17"/>
+    <mergeCell ref="K18:K20"/>
+    <mergeCell ref="H3:H7"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H11:H16"/>
+    <mergeCell ref="H18:H21"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="L3:L9"/>
+    <mergeCell ref="K3:K9"/>
+    <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="L11:L17"/>
-    <mergeCell ref="L18:L20"/>
-    <mergeCell ref="I3:I7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I11:I16"/>
-    <mergeCell ref="I18:I21"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
loaded material data from MagNet into MDB - 3C90, 3C92, 3C94, 3C95, 3E6, 3F4, N27, N30, N49, N87, T37 updated graphic showing overview of materials
</commit_message>
<xml_diff>
--- a/docs/source/figures/Material_Database_Overview.xlsx
+++ b/docs/source/figures/Material_Database_Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Repositorys\materialdatabase\docs\source\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D4E33C-F418-4CA9-BD9E-6D75B287A29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A6DD5A-90E3-4FE5-8F46-34205D0BF8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E51A1F85-B08D-41FE-9B94-BB5FD5A5BD95}"/>
   </bookViews>
@@ -345,7 +345,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,6 +407,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF92D050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -666,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -765,13 +771,64 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -780,61 +837,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1181,7 +1202,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1201,72 +1222,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="34"/>
+      <c r="F1" s="56"/>
       <c r="G1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="J1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="K1" s="52" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="44" t="s">
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="38"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="40"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="53"/>
     </row>
     <row r="3" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A3" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="48"/>
+      <c r="B3" s="37"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
       <c r="E3" s="25"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="45" t="s">
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="50" t="s">
         <v>26</v>
       </c>
       <c r="I3" s="10">
@@ -1275,7 +1296,7 @@
       <c r="J3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="36" t="s">
+      <c r="K3" s="48" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1283,20 +1304,20 @@
       <c r="A4" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="45"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="50"/>
       <c r="I4" s="11">
         <v>2200</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="36"/>
+      <c r="K4" s="48"/>
     </row>
     <row r="5" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A5" s="22" t="s">
@@ -1307,34 +1328,34 @@
       <c r="D5" s="30"/>
       <c r="E5" s="29"/>
       <c r="F5" s="29"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="45"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="50"/>
       <c r="I5" s="11">
         <v>1500</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="36"/>
+      <c r="K5" s="48"/>
     </row>
     <row r="6" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="45"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="50"/>
       <c r="I6" s="11">
         <v>800</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="36"/>
+      <c r="K6" s="48"/>
     </row>
     <row r="7" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A7" s="22" t="s">
@@ -1345,27 +1366,27 @@
       <c r="D7" s="19"/>
       <c r="E7" s="27"/>
       <c r="F7" s="30"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="45"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="50"/>
       <c r="I7" s="16">
         <v>2000</v>
       </c>
       <c r="J7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="36"/>
+      <c r="K7" s="48"/>
     </row>
     <row r="8" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="45" t="s">
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="50" t="s">
         <v>28</v>
       </c>
       <c r="I8" s="13">
@@ -1374,26 +1395,26 @@
       <c r="J8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="36"/>
+      <c r="K8" s="48"/>
     </row>
     <row r="9" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A9" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="45"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="50"/>
       <c r="I9" s="16">
         <v>6500</v>
       </c>
       <c r="J9" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="36"/>
+      <c r="K9" s="48"/>
     </row>
     <row r="10" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A10" s="33" t="s">
@@ -1405,7 +1426,7 @@
       <c r="E10" s="26"/>
       <c r="F10" s="26"/>
       <c r="G10" s="26"/>
-      <c r="H10" s="46" t="s">
+      <c r="H10" s="36" t="s">
         <v>25</v>
       </c>
       <c r="I10" s="14">
@@ -1422,13 +1443,13 @@
       <c r="A11" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
       <c r="E11" s="25"/>
-      <c r="F11" s="49"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="25"/>
-      <c r="H11" s="45" t="s">
+      <c r="H11" s="50" t="s">
         <v>25</v>
       </c>
       <c r="I11" s="13">
@@ -1437,7 +1458,7 @@
       <c r="J11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="41" t="s">
+      <c r="K11" s="47" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1445,20 +1466,20 @@
       <c r="A12" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="45"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="50"/>
       <c r="I12" s="11">
         <v>2300</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="36"/>
+      <c r="K12" s="48"/>
     </row>
     <row r="13" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A13" s="22" t="s">
@@ -1469,34 +1490,34 @@
       <c r="D13" s="19"/>
       <c r="E13" s="27"/>
       <c r="F13" s="29"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="45"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="50"/>
       <c r="I13" s="11">
         <v>1800</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K13" s="36"/>
+      <c r="K13" s="48"/>
     </row>
     <row r="14" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A14" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="52"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="45"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="50"/>
       <c r="I14" s="11">
         <v>2300</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K14" s="36"/>
+      <c r="K14" s="48"/>
     </row>
     <row r="15" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A15" s="22" t="s">
@@ -1507,48 +1528,48 @@
       <c r="D15" s="19"/>
       <c r="E15" s="27"/>
       <c r="F15" s="29"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="45"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="50"/>
       <c r="I15" s="11">
         <v>3000</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="36"/>
+      <c r="K15" s="48"/>
     </row>
     <row r="16" spans="1:15" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A16" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="45"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="50"/>
       <c r="I16" s="12">
         <v>900</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K16" s="36"/>
+      <c r="K16" s="48"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
     <row r="17" spans="1:11" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="46" t="s">
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="36" t="s">
         <v>29</v>
       </c>
       <c r="I17" s="6">
@@ -1557,19 +1578,19 @@
       <c r="J17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="36"/>
+      <c r="K17" s="48"/>
     </row>
     <row r="18" spans="1:11" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A18" s="57">
+      <c r="A18" s="46">
         <v>77</v>
       </c>
-      <c r="B18" s="48"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
       <c r="E18" s="25"/>
       <c r="F18" s="25"/>
       <c r="G18" s="25"/>
-      <c r="H18" s="47" t="s">
+      <c r="H18" s="51" t="s">
         <v>25</v>
       </c>
       <c r="I18" s="13">
@@ -1578,7 +1599,7 @@
       <c r="J18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="42" t="s">
+      <c r="K18" s="49" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1586,39 +1607,39 @@
       <c r="A19" s="23">
         <v>78</v>
       </c>
-      <c r="B19" s="52"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="47"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="51"/>
       <c r="I19" s="11">
         <v>2300</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K19" s="42"/>
+      <c r="K19" s="49"/>
     </row>
     <row r="20" spans="1:11" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A20" s="56">
+      <c r="A20" s="45">
         <v>79</v>
       </c>
-      <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="47"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="51"/>
       <c r="I20" s="12">
         <v>1400</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K20" s="42"/>
+      <c r="K20" s="49"/>
     </row>
     <row r="21" spans="1:11" ht="25.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A21" s="33" t="s">
@@ -1630,7 +1651,7 @@
       <c r="E21" s="26"/>
       <c r="F21" s="26"/>
       <c r="G21" s="26"/>
-      <c r="H21" s="47"/>
+      <c r="H21" s="51"/>
       <c r="I21" s="6">
         <v>1100</v>
       </c>
@@ -1649,12 +1670,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="K11:K17"/>
-    <mergeCell ref="K18:K20"/>
-    <mergeCell ref="H3:H7"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H11:H16"/>
-    <mergeCell ref="H18:H21"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="K3:K9"/>
@@ -1663,6 +1678,12 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="E1:F1"/>
+    <mergeCell ref="K11:K17"/>
+    <mergeCell ref="K18:K20"/>
+    <mergeCell ref="H3:H7"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H11:H16"/>
+    <mergeCell ref="H18:H21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>